<commit_message>
Updates , New Designs
</commit_message>
<xml_diff>
--- a/config/TestData.xlsx
+++ b/config/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/eclipse-workspace/KhibraWeb2/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A55A1D-B309-504E-B6D7-30BCC9694496}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F62D97-A066-4C4F-A731-4C03EE70F5BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="1400" windowWidth="26760" windowHeight="16600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6160" yWindow="1860" windowWidth="26760" windowHeight="16600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="219">
   <si>
     <t xml:space="preserve">Details </t>
   </si>
@@ -326,9 +326,6 @@
     <t xml:space="preserve">About Us </t>
   </si>
   <si>
-    <t>This University is the best in the World</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
@@ -687,6 +684,21 @@
   </si>
   <si>
     <t>ade</t>
+  </si>
+  <si>
+    <t>Updated University Name</t>
+  </si>
+  <si>
+    <t>Abilene University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This University is the best in the World .   Move Ahead </t>
+  </si>
+  <si>
+    <t>Employer Name Update</t>
+  </si>
+  <si>
+    <t>Google Nigeria</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1093,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1130,7 +1142,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1297,7 +1309,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D8">
         <v>71</v>
@@ -1341,7 +1353,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D12">
         <v>111</v>
@@ -1382,10 +1394,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16">
         <v>151</v>
@@ -1393,10 +1405,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17">
         <v>161</v>
@@ -1480,7 +1492,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4">
         <v>31</v>
@@ -1535,7 +1547,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D9">
         <v>81</v>
@@ -1634,7 +1646,7 @@
         <v>67</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D18">
         <v>171</v>
@@ -1664,7 +1676,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -1732,7 +1744,7 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1744,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18A30B1-3DDD-494C-A1AA-F01927EDDBCB}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1775,10 +1787,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="C3">
         <v>21</v>
@@ -1786,10 +1798,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4">
         <v>31</v>
@@ -1797,10 +1809,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5">
         <v>41</v>
@@ -1808,10 +1820,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6">
         <v>51</v>
@@ -1819,10 +1831,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="C7">
         <v>61</v>
@@ -1830,10 +1842,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C8">
         <v>71</v>
@@ -1841,10 +1853,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9">
         <v>81</v>
@@ -1852,7 +1864,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>9</v>
@@ -1863,7 +1875,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -1874,10 +1886,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C12">
         <v>111</v>
@@ -1885,10 +1897,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="C13">
         <v>121</v>
@@ -1937,10 +1949,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1959,7 +1971,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -2027,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6845A69-C50C-F84F-A7A3-F8D6A1433EE3}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2128,7 +2140,7 @@
         <v>93</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>94</v>
+        <v>216</v>
       </c>
       <c r="C9" s="6">
         <v>81</v>
@@ -2136,10 +2148,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="C10" s="6">
         <v>91</v>
@@ -2147,10 +2159,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="6">
         <v>101</v>
@@ -2158,10 +2170,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -2169,10 +2181,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -2180,10 +2192,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -2191,10 +2203,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -2202,10 +2214,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="6">
         <v>15</v>
@@ -2213,10 +2225,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="6">
         <v>16</v>
@@ -2224,10 +2236,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="6">
         <v>17</v>
@@ -2235,10 +2247,10 @@
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" s="6">
         <v>18</v>
@@ -2246,10 +2258,10 @@
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="6">
         <v>19</v>
@@ -2257,10 +2269,10 @@
     </row>
     <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" s="6">
         <v>20</v>
@@ -2268,7 +2280,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>77</v>
@@ -2279,10 +2291,10 @@
     </row>
     <row r="23" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="C23" s="6">
         <v>22</v>
@@ -2290,10 +2302,10 @@
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>122</v>
       </c>
       <c r="C24" s="6">
         <v>23</v>
@@ -2301,17 +2313,22 @@
     </row>
     <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C25" s="6">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="11"/>
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>215</v>
+      </c>
       <c r="C26" s="6">
         <v>25</v>
       </c>
@@ -2356,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B52A2B0-C354-904C-8F20-4044151A34A9}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2377,10 +2394,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>2</v>
@@ -2388,10 +2405,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6">
         <v>21</v>
@@ -2399,10 +2416,10 @@
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="6">
         <v>31</v>
@@ -2410,10 +2427,10 @@
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="6">
         <v>41</v>
@@ -2421,10 +2438,10 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" s="6">
         <v>51</v>
@@ -2432,10 +2449,10 @@
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>138</v>
       </c>
       <c r="C7" s="6">
         <v>61</v>
@@ -2443,10 +2460,10 @@
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="6">
         <v>71</v>
@@ -2454,10 +2471,10 @@
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="6">
         <v>81</v>
@@ -2465,10 +2482,10 @@
     </row>
     <row r="10" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="C10" s="6">
         <v>91</v>
@@ -2476,10 +2493,10 @@
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -2487,10 +2504,10 @@
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -2498,10 +2515,10 @@
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -2509,7 +2526,7 @@
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>92</v>
@@ -2520,10 +2537,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -2531,10 +2548,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="C16" s="6">
         <v>15</v>
@@ -2542,10 +2559,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="6">
         <v>16</v>
@@ -2553,10 +2570,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="C18" s="6">
         <v>17</v>
@@ -2564,7 +2581,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>81</v>
@@ -2575,7 +2592,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>91</v>
@@ -2586,10 +2603,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C21" s="6">
         <v>20</v>
@@ -2597,10 +2614,10 @@
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" s="6">
         <v>21</v>
@@ -2608,10 +2625,10 @@
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="C23" s="6">
         <v>22</v>
@@ -2619,10 +2636,10 @@
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C24" s="6">
         <v>23</v>
@@ -2630,10 +2647,10 @@
     </row>
     <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>169</v>
       </c>
       <c r="C25" s="6">
         <v>24</v>
@@ -2641,7 +2658,7 @@
     </row>
     <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>24</v>
@@ -2652,10 +2669,10 @@
     </row>
     <row r="27" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>173</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="C27" s="6">
         <v>26</v>
@@ -2663,10 +2680,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>176</v>
       </c>
       <c r="C28" s="6">
         <v>27</v>
@@ -2674,7 +2691,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
         <v>51</v>
@@ -2685,10 +2702,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C30" s="6">
         <v>29</v>
@@ -2696,10 +2713,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C31" s="6">
         <v>30</v>
@@ -2707,27 +2724,32 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C32" s="6">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>218</v>
+      </c>
       <c r="C33" s="6">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C34" s="6">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C35" s="6">
         <v>34</v>
       </c>

</xml_diff>